<commit_message>
added box for carcass
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/dsi/recap.xlsx
+++ b/CustomLabelPrinter/src/paperwork/dsi/recap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\dsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E483468E-D16F-4900-85AC-61B642FFAF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E83FC4-8EBE-420D-BDBC-14978F628A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -149,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +253,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -542,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -591,9 +609,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -703,6 +718,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -732,6 +765,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,54 +1072,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1110,10 +1152,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="49"/>
+      <c r="P4" s="46"/>
       <c r="R4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1914,57 +1956,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="7"/>
       <c r="S2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1997,10 +2039,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="49"/>
+      <c r="P4" s="46"/>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -2783,8 +2825,8 @@
   </sheetPr>
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A35" zoomScale="50" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2795,54 +2837,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -2875,20 +2917,20 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="49"/>
+      <c r="P4" s="46"/>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="54">
+      <c r="C5" s="51">
         <v>21102</v>
       </c>
-      <c r="D5" s="55"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2899,13 +2941,13 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="57"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="54"/>
     </row>
     <row r="6" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2916,13 +2958,13 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="59"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="56"/>
     </row>
     <row r="7" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2933,13 +2975,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="61"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="58"/>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -2950,13 +2992,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="61"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="58"/>
     </row>
     <row r="9" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -2967,13 +3009,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="61"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="58"/>
     </row>
     <row r="10" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -2984,13 +3026,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="61"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="58"/>
     </row>
     <row r="11" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -3001,13 +3043,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="61"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="58"/>
     </row>
     <row r="12" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -3018,13 +3060,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="61"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="58"/>
     </row>
     <row r="13" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="51"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -3035,13 +3077,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="58"/>
     </row>
     <row r="14" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -3052,13 +3094,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="61"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="58"/>
     </row>
     <row r="15" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -3071,13 +3113,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="61"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="58"/>
     </row>
     <row r="16" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="48"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -3088,13 +3130,13 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="61"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="58"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
@@ -3105,13 +3147,13 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="61"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="58"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3122,13 +3164,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="61"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="58"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -3139,13 +3181,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="61"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="58"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3156,13 +3198,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="61"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="58"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3173,13 +3215,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="61"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="58"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3190,13 +3232,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="61"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="58"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -3207,13 +3249,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="61"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="58"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="51"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3224,13 +3266,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="61"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="58"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -3241,13 +3283,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="61"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="58"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3258,13 +3300,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="61"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="58"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3275,13 +3317,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="62"/>
-      <c r="P27" s="63"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="60"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="52"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -3292,13 +3334,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="65"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="62"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -3309,13 +3351,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="66"/>
-      <c r="P29" s="67"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="64"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -3326,13 +3368,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="66"/>
-      <c r="P30" s="67"/>
+      <c r="O30" s="63"/>
+      <c r="P30" s="64"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3343,13 +3385,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="66"/>
-      <c r="P31" s="67"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="64"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="51"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -3360,13 +3402,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="66"/>
-      <c r="P32" s="67"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="64"/>
     </row>
     <row r="33" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="51"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -3377,13 +3419,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="66"/>
-      <c r="P33" s="67"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="64"/>
     </row>
     <row r="34" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="51"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3394,13 +3436,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="66"/>
-      <c r="P34" s="67"/>
+      <c r="O34" s="63"/>
+      <c r="P34" s="64"/>
     </row>
     <row r="35" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -3411,13 +3453,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="67"/>
+      <c r="O35" s="63"/>
+      <c r="P35" s="64"/>
     </row>
     <row r="36" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="51"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -3428,13 +3470,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="67"/>
+      <c r="O36" s="63"/>
+      <c r="P36" s="64"/>
     </row>
     <row r="37" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="51"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -3445,13 +3487,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="67"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="64"/>
     </row>
     <row r="38" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="53"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -3462,26 +3504,28 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="68"/>
-      <c r="P38" s="69"/>
+      <c r="O38" s="65"/>
+      <c r="P38" s="66"/>
     </row>
     <row r="39" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="70"/>
-      <c r="P39" s="71"/>
+      <c r="C39" s="67">
+        <v>10468</v>
+      </c>
+      <c r="D39" s="68"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="84"/>
+      <c r="K39" s="84"/>
+      <c r="L39" s="84"/>
+      <c r="M39" s="84"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="74"/>
       <c r="Q39"/>
       <c r="R39"/>
       <c r="S39"/>
@@ -3489,20 +3533,20 @@
     <row r="40" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="72"/>
-      <c r="P40" s="73"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="84"/>
+      <c r="I40" s="84"/>
+      <c r="J40" s="84"/>
+      <c r="K40" s="84"/>
+      <c r="L40" s="84"/>
+      <c r="M40" s="84"/>
+      <c r="N40" s="85"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="76"/>
       <c r="Q40"/>
       <c r="R40"/>
       <c r="S40"/>
@@ -3510,20 +3554,20 @@
     <row r="41" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="72"/>
-      <c r="P41" s="73"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="83"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="84"/>
+      <c r="L41" s="84"/>
+      <c r="M41" s="84"/>
+      <c r="N41" s="85"/>
+      <c r="O41" s="75"/>
+      <c r="P41" s="76"/>
       <c r="Q41"/>
       <c r="R41"/>
       <c r="S41"/>
@@ -3531,20 +3575,20 @@
     <row r="42" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="30"/>
-      <c r="O42" s="72"/>
-      <c r="P42" s="73"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="83"/>
+      <c r="F42" s="84"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="84"/>
+      <c r="I42" s="84"/>
+      <c r="J42" s="84"/>
+      <c r="K42" s="84"/>
+      <c r="L42" s="84"/>
+      <c r="M42" s="84"/>
+      <c r="N42" s="85"/>
+      <c r="O42" s="75"/>
+      <c r="P42" s="76"/>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
@@ -3552,20 +3596,20 @@
     <row r="43" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
-      <c r="C43" s="74"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="30"/>
-      <c r="O43" s="74"/>
-      <c r="P43" s="75"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="83"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="84"/>
+      <c r="I43" s="84"/>
+      <c r="J43" s="84"/>
+      <c r="K43" s="84"/>
+      <c r="L43" s="84"/>
+      <c r="M43" s="84"/>
+      <c r="N43" s="85"/>
+      <c r="O43" s="77"/>
+      <c r="P43" s="78"/>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
@@ -3728,241 +3772,241 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="31" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" style="31" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="31" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" style="31" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="6.28515625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="28" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="28" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="28" customWidth="1"/>
+    <col min="6" max="9" width="8.85546875" style="28" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="34"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="31"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="33"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77" t="s">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77" t="s">
+      <c r="D13" s="80"/>
+      <c r="E13" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77" t="s">
+      <c r="G13" s="80"/>
+      <c r="H13" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="77"/>
+      <c r="I13" s="80"/>
     </row>
     <row r="14" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
     </row>
     <row r="16" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="77"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="77"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
     </row>
     <row r="18" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="77" t="s">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
     </row>
     <row r="20" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
     </row>
     <row r="22" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
     </row>
     <row r="24" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="77"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
+      <c r="A24" s="80"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
     </row>
     <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="77"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="77"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="80"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="38">
@@ -4020,288 +4064,288 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="31" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="31" customWidth="1"/>
-    <col min="4" max="5" width="6.7109375" style="31" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="31" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="14.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="28" customWidth="1"/>
+    <col min="4" max="5" width="6.7109375" style="28" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="28" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="G3" s="78" t="s">
+      <c r="B3" s="81"/>
+      <c r="G3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="39"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="36"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="42"/>
-      <c r="C7" s="39"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="36"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="44"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="41"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="42"/>
-      <c r="C9" s="39"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="36"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="42"/>
-      <c r="C10" s="39"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="36"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="39"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="36"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="42"/>
-      <c r="C12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="36"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="42"/>
-      <c r="C13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="36"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="42"/>
-      <c r="C14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="36"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="42"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="39"/>
-      <c r="G16" s="43" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="36"/>
+      <c r="G16" s="40" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="42"/>
-      <c r="C17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="36"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="42"/>
-      <c r="C18" s="39"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="36"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B19" s="42"/>
-      <c r="C19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="36"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B20" s="42"/>
-      <c r="C20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="36"/>
     </row>
     <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="36"/>
     </row>
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B22" s="42"/>
-      <c r="C22" s="39"/>
-      <c r="G22" s="78" t="s">
+      <c r="B22" s="39"/>
+      <c r="C22" s="36"/>
+      <c r="G22" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="81"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B23" s="42"/>
-      <c r="C23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="36"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="42"/>
-      <c r="C24" s="39"/>
-      <c r="G24" s="31" t="s">
+      <c r="B24" s="39"/>
+      <c r="C24" s="36"/>
+      <c r="G24" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="42"/>
-      <c r="C25" s="39"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="36"/>
     </row>
     <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="39"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="36"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B27" s="42"/>
-      <c r="C27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="36"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B28" s="42"/>
-      <c r="C28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="36"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B29" s="42"/>
-      <c r="C29" s="39"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="36"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B30" s="42"/>
-      <c r="C30" s="39"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="36"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
     </row>
     <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="39"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="36"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B32" s="42"/>
-      <c r="C32" s="39"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="36"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B33" s="42"/>
-      <c r="C33" s="39"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="36"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B34" s="42"/>
-      <c r="C34" s="39"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="36"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="42"/>
-      <c r="C35" s="39"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="36"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
     </row>
     <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="39"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="36"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B37" s="42"/>
-      <c r="C37" s="39"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="36"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="42"/>
-      <c r="C38" s="39"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="36"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B39" s="42"/>
-      <c r="C39" s="39"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="36"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B40" s="42"/>
-      <c r="C40" s="39"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="36"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
     </row>
     <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B41" s="42"/>
-      <c r="C41" s="39"/>
-      <c r="G41" s="40" t="s">
+      <c r="B41" s="39"/>
+      <c r="C41" s="36"/>
+      <c r="G41" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="H41" s="41"/>
+      <c r="H41" s="38"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B42" s="42"/>
-      <c r="C42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="36"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B43" s="42"/>
-      <c r="C43" s="39"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="36"/>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B44" s="42"/>
-      <c r="C44" s="39"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="36"/>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>